<commit_message>
spreadsheets: Remove options from project "stage of development"
Schema changes were done in a7590e362efb17aeb54092e28cff2ec27586354d

(This should have been done there too)
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_public_v016.xlsx
+++ b/indigo/spreadsheetform_guides/project_public_v016.xlsx
@@ -10332,9 +10332,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -11273,7 +11273,7 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C17" type="list">
       <formula1>"YES,NO"</formula1>
       <formula2>0</formula2>
@@ -11288,6 +11288,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C20" type="none">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C14" type="list">
+      <formula1>"Contracted,Implementation,Service delivery complete,Complete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>